<commit_message>
Podstrany pre veduceho pracoviska
</commit_message>
<xml_diff>
--- a/Architektura/website_architecture_list.xlsx
+++ b/Architektura/website_architecture_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentukfsk-my.sharepoint.com/personal/marek_hrabcak_student_ukf_sk/Documents/Mgr/SoftveroveInzinierstvo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrabcak/github/SI/Architektura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{1FB0AC79-725B-EF45-AF1E-0523DCC231B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38D3E216-726D-F94F-8447-0CB8F840B32F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4515FD7-3848-F344-BAE0-43E0FECE5788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
+    <workbookView xWindow="21840" yWindow="500" windowWidth="16560" windowHeight="21100" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="188">
   <si>
     <t>HOME</t>
   </si>
@@ -407,9 +407,6 @@
     <t>headReportList</t>
   </si>
   <si>
-    <t>headReportCreate</t>
-  </si>
-  <si>
     <t>headReportUpd</t>
   </si>
   <si>
@@ -467,15 +464,9 @@
     <t>respFeedDel</t>
   </si>
   <si>
-    <t>headrespList</t>
-  </si>
-  <si>
     <t>respReportRead</t>
   </si>
   <si>
-    <t>headrespUpd</t>
-  </si>
-  <si>
     <t>respReportAdd</t>
   </si>
   <si>
@@ -597,6 +588,18 @@
   </si>
   <si>
     <t>cmpRegDetail</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>headRespList</t>
+  </si>
+  <si>
+    <t>headRespUpd</t>
+  </si>
+  <si>
+    <t>headReportAdd</t>
   </si>
 </sst>
 </file>
@@ -612,12 +615,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -632,8 +641,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,10 +659,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -952,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5B7B27-9C0C-C145-A167-201B91E0FE9A}">
-  <dimension ref="B1:AT51"/>
+  <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AT5" sqref="AT5"/>
+    <sheetView tabSelected="1" topLeftCell="N2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,12 +982,15 @@
     <col min="45" max="45" width="2.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="Y1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1004,18 +1013,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
         <v>129</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" t="s">
-        <v>130</v>
       </c>
       <c r="K5" t="s">
         <v>63</v>
@@ -1032,7 +1041,7 @@
       <c r="U5" t="s">
         <v>72</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="1" t="s">
         <v>118</v>
       </c>
       <c r="Y5" t="s">
@@ -1042,7 +1051,7 @@
         <v>72</v>
       </c>
       <c r="AD5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AG5" t="s">
         <v>15</v>
@@ -1051,7 +1060,7 @@
         <v>72</v>
       </c>
       <c r="AL5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AO5" t="s">
         <v>21</v>
@@ -1060,10 +1069,10 @@
         <v>72</v>
       </c>
       <c r="AT5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="2:46" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1091,7 @@
       <c r="U7" t="s">
         <v>72</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="1" t="s">
         <v>119</v>
       </c>
       <c r="Z7" t="s">
@@ -1092,7 +1101,7 @@
         <v>73</v>
       </c>
       <c r="AD7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AH7" t="s">
         <v>54</v>
@@ -1101,7 +1110,7 @@
         <v>73</v>
       </c>
       <c r="AL7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AP7" t="s">
         <v>45</v>
@@ -1110,10 +1119,10 @@
         <v>73</v>
       </c>
       <c r="AT7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="2:46" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>71</v>
       </c>
@@ -1132,7 +1141,7 @@
       <c r="U9" t="s">
         <v>72</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="1" t="s">
         <v>120</v>
       </c>
       <c r="Z9" t="s">
@@ -1142,7 +1151,7 @@
         <v>74</v>
       </c>
       <c r="AD9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AH9" t="s">
         <v>37</v>
@@ -1151,7 +1160,7 @@
         <v>74</v>
       </c>
       <c r="AL9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AP9" t="s">
         <v>46</v>
@@ -1160,10 +1169,10 @@
         <v>74</v>
       </c>
       <c r="AT9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="2:46" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="L11" t="s">
         <v>64</v>
       </c>
@@ -1179,7 +1188,7 @@
       <c r="U11" t="s">
         <v>72</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V11" s="1" t="s">
         <v>121</v>
       </c>
       <c r="Z11" t="s">
@@ -1189,7 +1198,7 @@
         <v>80</v>
       </c>
       <c r="AD11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AH11" t="s">
         <v>91</v>
@@ -1198,7 +1207,7 @@
         <v>80</v>
       </c>
       <c r="AL11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AO11" t="s">
         <v>24</v>
@@ -1207,10 +1216,10 @@
         <v>72</v>
       </c>
       <c r="AT11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="2:46" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="L13" t="s">
         <v>79</v>
       </c>
@@ -1226,7 +1235,7 @@
       <c r="U13" t="s">
         <v>72</v>
       </c>
-      <c r="V13" t="s">
+      <c r="V13" s="1" t="s">
         <v>122</v>
       </c>
       <c r="Y13" t="s">
@@ -1236,7 +1245,7 @@
         <v>72</v>
       </c>
       <c r="AD13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AG13" t="s">
         <v>16</v>
@@ -1245,7 +1254,7 @@
         <v>72</v>
       </c>
       <c r="AL13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AP13" t="s">
         <v>47</v>
@@ -1254,10 +1263,10 @@
         <v>73</v>
       </c>
       <c r="AT13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="2:46" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="L15" t="s">
         <v>66</v>
       </c>
@@ -1273,8 +1282,8 @@
       <c r="U15" t="s">
         <v>73</v>
       </c>
-      <c r="V15" t="s">
-        <v>123</v>
+      <c r="V15" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="Z15" t="s">
         <v>31</v>
@@ -1283,7 +1292,7 @@
         <v>74</v>
       </c>
       <c r="AD15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AH15" t="s">
         <v>55</v>
@@ -1292,7 +1301,7 @@
         <v>73</v>
       </c>
       <c r="AL15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AP15" t="s">
         <v>27</v>
@@ -1301,7 +1310,7 @@
         <v>74</v>
       </c>
       <c r="AT15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="11:46" x14ac:dyDescent="0.2">
@@ -1320,8 +1329,8 @@
       <c r="U17" t="s">
         <v>74</v>
       </c>
-      <c r="V17" t="s">
-        <v>124</v>
+      <c r="V17" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="Y17" t="s">
         <v>12</v>
@@ -1330,7 +1339,7 @@
         <v>72</v>
       </c>
       <c r="AD17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH17" t="s">
         <v>56</v>
@@ -1339,7 +1348,7 @@
         <v>74</v>
       </c>
       <c r="AL17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AO17" t="s">
         <v>22</v>
@@ -1348,7 +1357,7 @@
         <v>72</v>
       </c>
       <c r="AT17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="11:46" x14ac:dyDescent="0.2">
@@ -1368,7 +1377,7 @@
         <v>80</v>
       </c>
       <c r="V19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z19" t="s">
         <v>33</v>
@@ -1377,7 +1386,7 @@
         <v>73</v>
       </c>
       <c r="AD19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AH19" t="s">
         <v>92</v>
@@ -1386,7 +1395,7 @@
         <v>80</v>
       </c>
       <c r="AL19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AP19" t="s">
         <v>48</v>
@@ -1395,7 +1404,7 @@
         <v>74</v>
       </c>
       <c r="AT19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="11:46" x14ac:dyDescent="0.2">
@@ -1414,8 +1423,8 @@
       <c r="U21" t="s">
         <v>72</v>
       </c>
-      <c r="V21" t="s">
-        <v>126</v>
+      <c r="V21" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="Z21" t="s">
         <v>34</v>
@@ -1424,7 +1433,7 @@
         <v>74</v>
       </c>
       <c r="AD21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AG21" t="s">
         <v>17</v>
@@ -1433,7 +1442,7 @@
         <v>72</v>
       </c>
       <c r="AL21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AO21" t="s">
         <v>23</v>
@@ -1442,7 +1451,7 @@
         <v>72</v>
       </c>
       <c r="AT21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="11:46" x14ac:dyDescent="0.2">
@@ -1461,17 +1470,17 @@
       <c r="U23" t="s">
         <v>72</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z23" t="s">
         <v>127</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>128</v>
       </c>
       <c r="AC23" t="s">
         <v>80</v>
       </c>
       <c r="AD23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AH23" t="s">
         <v>57</v>
@@ -1480,7 +1489,7 @@
         <v>73</v>
       </c>
       <c r="AL23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AP23" t="s">
         <v>47</v>
@@ -1489,7 +1498,7 @@
         <v>73</v>
       </c>
       <c r="AT23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="11:46" x14ac:dyDescent="0.2">
@@ -1508,8 +1517,8 @@
       <c r="U25" t="s">
         <v>72</v>
       </c>
-      <c r="V25" t="s">
-        <v>143</v>
+      <c r="V25" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="Y25" t="s">
         <v>13</v>
@@ -1518,7 +1527,7 @@
         <v>72</v>
       </c>
       <c r="AD25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AH25" t="s">
         <v>58</v>
@@ -1527,7 +1536,7 @@
         <v>74</v>
       </c>
       <c r="AL25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AP25" t="s">
         <v>27</v>
@@ -1536,7 +1545,7 @@
         <v>74</v>
       </c>
       <c r="AT25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="11:46" x14ac:dyDescent="0.2">
@@ -1555,8 +1564,8 @@
       <c r="U27" t="s">
         <v>74</v>
       </c>
-      <c r="V27" t="s">
-        <v>145</v>
+      <c r="V27" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="Z27" t="s">
         <v>51</v>
@@ -1565,7 +1574,7 @@
         <v>73</v>
       </c>
       <c r="AD27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AH27" t="s">
         <v>93</v>
@@ -1574,16 +1583,16 @@
         <v>80</v>
       </c>
       <c r="AL27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AP27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AS27" t="s">
         <v>80</v>
       </c>
       <c r="AT27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="11:46" x14ac:dyDescent="0.2">
@@ -1603,7 +1612,7 @@
         <v>74</v>
       </c>
       <c r="AD29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AG29" t="s">
         <v>18</v>
@@ -1612,7 +1621,7 @@
         <v>72</v>
       </c>
       <c r="AL29" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="11:46" x14ac:dyDescent="0.2">
@@ -1632,7 +1641,7 @@
         <v>80</v>
       </c>
       <c r="AD31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AH31" t="s">
         <v>59</v>
@@ -1641,7 +1650,7 @@
         <v>74</v>
       </c>
       <c r="AL31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="11:38" x14ac:dyDescent="0.2">
@@ -1661,7 +1670,7 @@
         <v>72</v>
       </c>
       <c r="AD33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AG33" t="s">
         <v>19</v>
@@ -1670,7 +1679,7 @@
         <v>72</v>
       </c>
       <c r="AL33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="11:38" x14ac:dyDescent="0.2">
@@ -1690,7 +1699,7 @@
         <v>74</v>
       </c>
       <c r="AD35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AH35" t="s">
         <v>60</v>
@@ -1699,7 +1708,7 @@
         <v>73</v>
       </c>
       <c r="AL35" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="11:38" x14ac:dyDescent="0.2">
@@ -1719,7 +1728,7 @@
         <v>72</v>
       </c>
       <c r="AD37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AH37" t="s">
         <v>61</v>
@@ -1728,7 +1737,7 @@
         <v>74</v>
       </c>
       <c r="AL37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="11:38" x14ac:dyDescent="0.2">
@@ -1748,7 +1757,7 @@
         <v>73</v>
       </c>
       <c r="AD39" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AH39" t="s">
         <v>94</v>
@@ -1757,12 +1766,12 @@
         <v>80</v>
       </c>
       <c r="AL39" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="11:38" x14ac:dyDescent="0.2">
       <c r="K41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M41" t="s">
         <v>72</v>
@@ -1777,7 +1786,7 @@
         <v>72</v>
       </c>
       <c r="AD41" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AG41" t="s">
         <v>20</v>
@@ -1786,7 +1795,7 @@
         <v>72</v>
       </c>
       <c r="AL41" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="11:38" x14ac:dyDescent="0.2">
@@ -1806,7 +1815,7 @@
         <v>73</v>
       </c>
       <c r="AD43" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="11:38" x14ac:dyDescent="0.2">
@@ -1826,7 +1835,7 @@
         <v>74</v>
       </c>
       <c r="AD45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="11:38" x14ac:dyDescent="0.2">
@@ -1846,7 +1855,7 @@
         <v>80</v>
       </c>
       <c r="AD47" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="11:14" x14ac:dyDescent="0.2">
@@ -1862,7 +1871,7 @@
     </row>
     <row r="51" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M51" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Aktualizacia dokumentu s aplikacnou architekturou
</commit_message>
<xml_diff>
--- a/Architektura/website_architecture_list.xlsx
+++ b/Architektura/website_architecture_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrabcak/github/SI/Architektura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4515FD7-3848-F344-BAE0-43E0FECE5788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ECB46C-9649-9B49-A2CF-7D4E973AB4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21840" yWindow="500" windowWidth="16560" windowHeight="21100" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
   </bookViews>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5B7B27-9C0C-C145-A167-201B91E0FE9A}">
   <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1882,5 +1882,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update stranok veduceho pracoviska
</commit_message>
<xml_diff>
--- a/Architektura/website_architecture_list.xlsx
+++ b/Architektura/website_architecture_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrabcak/github/SI/Architektura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ECB46C-9649-9B49-A2CF-7D4E973AB4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E1AA81-22CB-F040-A292-F093F1F4069B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="500" windowWidth="16560" windowHeight="21100" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="190">
   <si>
     <t>HOME</t>
   </si>
@@ -600,6 +600,12 @@
   </si>
   <si>
     <t>headReportAdd</t>
+  </si>
+  <si>
+    <t>Pridanie povereného pracovníka pracoviska</t>
+  </si>
+  <si>
+    <t>headRespAdd</t>
   </si>
 </sst>
 </file>
@@ -960,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5B7B27-9C0C-C145-A167-201B91E0FE9A}">
   <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:Q25"/>
+    <sheetView tabSelected="1" topLeftCell="N17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1605,6 +1611,15 @@
       <c r="N29" t="s">
         <v>105</v>
       </c>
+      <c r="R29" t="s">
+        <v>188</v>
+      </c>
+      <c r="U29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="Z29" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Podstránky pre Zástupca firmy a organizácie + navbar
</commit_message>
<xml_diff>
--- a/Architektura/website_architecture_list.xlsx
+++ b/Architektura/website_architecture_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Project_SI\Architektura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E208F8-9F1C-40D2-978E-0B62DBA06C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B37198F-418D-4073-A9F5-4B271A68D6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="3150" windowWidth="21600" windowHeight="11505" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,6 +640,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -653,10 +659,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -973,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5B7B27-9C0C-C145-A167-201B91E0FE9A}">
   <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN27" sqref="AN27"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AX29" sqref="AX29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1087,7 @@
       <c r="AS5" t="s">
         <v>72</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AT5" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1227,7 +1234,7 @@
       <c r="AS11" t="s">
         <v>72</v>
       </c>
-      <c r="AT11" t="s">
+      <c r="AT11" s="1" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1265,7 +1272,7 @@
       <c r="AK13" t="s">
         <v>72</v>
       </c>
-      <c r="AL13" s="1" t="s">
+      <c r="AL13" s="3" t="s">
         <v>156</v>
       </c>
       <c r="AP13" t="s">
@@ -1274,7 +1281,7 @@
       <c r="AS13" t="s">
         <v>73</v>
       </c>
-      <c r="AT13" t="s">
+      <c r="AT13" s="1" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1312,7 +1319,7 @@
       <c r="AK15" t="s">
         <v>73</v>
       </c>
-      <c r="AL15" s="1" t="s">
+      <c r="AL15" s="3" t="s">
         <v>157</v>
       </c>
       <c r="AP15" t="s">
@@ -1321,7 +1328,7 @@
       <c r="AS15" t="s">
         <v>74</v>
       </c>
-      <c r="AT15" t="s">
+      <c r="AT15" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1359,7 +1366,7 @@
       <c r="AK17" t="s">
         <v>74</v>
       </c>
-      <c r="AL17" s="1" t="s">
+      <c r="AL17" s="3" t="s">
         <v>158</v>
       </c>
       <c r="AO17" t="s">
@@ -1368,7 +1375,7 @@
       <c r="AS17" t="s">
         <v>72</v>
       </c>
-      <c r="AT17" t="s">
+      <c r="AT17" s="1" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1415,7 +1422,7 @@
       <c r="AS19" t="s">
         <v>74</v>
       </c>
-      <c r="AT19" t="s">
+      <c r="AT19" s="1" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1462,7 +1469,7 @@
       <c r="AS21" t="s">
         <v>72</v>
       </c>
-      <c r="AT21" t="s">
+      <c r="AT21" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1509,7 +1516,7 @@
       <c r="AS23" t="s">
         <v>73</v>
       </c>
-      <c r="AT23" t="s">
+      <c r="AT23" s="1" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1556,7 +1563,7 @@
       <c r="AS25" t="s">
         <v>74</v>
       </c>
-      <c r="AT25" t="s">
+      <c r="AT25" s="1" t="s">
         <v>181</v>
       </c>
     </row>

</xml_diff>

<commit_message>
oprava firma a person add
</commit_message>
<xml_diff>
--- a/Architektura/website_architecture_list.xlsx
+++ b/Architektura/website_architecture_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Project_SI\Architektura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\PhpstormProjects\Project_SI\Architektura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B37198F-418D-4073-A9F5-4B271A68D6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA2F7A-641C-4050-B116-09EBE90D3B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
+    <workbookView minimized="1" xWindow="1080" yWindow="1080" windowWidth="15432" windowHeight="8508" xr2:uid="{C4DA45A7-D938-0747-83AB-FECF0C752D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -980,28 +980,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5B7B27-9C0C-C145-A167-201B91E0FE9A}">
   <dimension ref="A1:AT51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AX29" sqref="AX29"/>
+    <sheetView tabSelected="1" topLeftCell="F11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="2.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="26.25" customWidth="1"/>
+    <col min="7" max="7" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="26.19921875" customWidth="1"/>
     <col min="13" max="13" width="2.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.3984375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.09765625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="3.5" customWidth="1"/>
-    <col min="33" max="33" width="5.25" customWidth="1"/>
+    <col min="33" max="33" width="5.19921875" customWidth="1"/>
     <col min="37" max="37" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.75" customWidth="1"/>
+    <col min="40" max="40" width="5.69921875" customWidth="1"/>
     <col min="41" max="41" width="8.5" customWidth="1"/>
     <col min="45" max="45" width="2.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1093,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>71</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="L11" t="s">
         <v>64</v>
       </c>
@@ -1238,7 +1240,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="L13" t="s">
         <v>79</v>
       </c>
@@ -1285,7 +1287,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="L15" t="s">
         <v>66</v>
       </c>
@@ -1332,7 +1334,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:46" x14ac:dyDescent="0.3">
       <c r="L17" t="s">
         <v>67</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:46" x14ac:dyDescent="0.3">
       <c r="L19" t="s">
         <v>81</v>
       </c>
@@ -1426,7 +1428,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="11:46" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
         <v>76</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:46" x14ac:dyDescent="0.3">
       <c r="L23" t="s">
         <v>78</v>
       </c>
@@ -1520,7 +1522,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:46" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>75</v>
       </c>
@@ -1567,7 +1569,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="11:46" x14ac:dyDescent="0.3">
       <c r="L27" t="s">
         <v>77</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="11:46" x14ac:dyDescent="0.3">
       <c r="L29" t="s">
         <v>68</v>
       </c>
@@ -1652,7 +1654,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="11:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="11:46" x14ac:dyDescent="0.3">
       <c r="L31" t="s">
         <v>82</v>
       </c>
@@ -1681,7 +1683,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:38" x14ac:dyDescent="0.3">
       <c r="K33" t="s">
         <v>26</v>
       </c>
@@ -1710,7 +1712,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:38" x14ac:dyDescent="0.3">
       <c r="L35" t="s">
         <v>69</v>
       </c>
@@ -1739,7 +1741,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:38" x14ac:dyDescent="0.3">
       <c r="L37" t="s">
         <v>70</v>
       </c>
@@ -1768,7 +1770,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:38" x14ac:dyDescent="0.3">
       <c r="L39" t="s">
         <v>83</v>
       </c>
@@ -1797,7 +1799,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:38" x14ac:dyDescent="0.3">
       <c r="K41" t="s">
         <v>130</v>
       </c>
@@ -1826,7 +1828,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:38" x14ac:dyDescent="0.3">
       <c r="K43" t="s">
         <v>28</v>
       </c>
@@ -1846,7 +1848,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:38" x14ac:dyDescent="0.3">
       <c r="L45" t="s">
         <v>3</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="11:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="11:38" x14ac:dyDescent="0.3">
       <c r="L47" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1888,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:14" x14ac:dyDescent="0.3">
       <c r="L49" t="s">
         <v>84</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K51" t="s">
         <v>131</v>
       </c>

</xml_diff>